<commit_message>
Made work at home
put mongod into release folder
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Release/Subject 5 - Roiy pilot.xlsx
+++ b/FilmFinder/FilmFinder/bin/Release/Subject 5 - Roiy pilot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="27795" windowHeight="12585"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Subject 5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -594,7 +594,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -679,11 +679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40565376"/>
-        <c:axId val="44810624"/>
+        <c:axId val="121938304"/>
+        <c:axId val="121939840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40565376"/>
+        <c:axId val="121938304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44810624"/>
+        <c:crossAx val="121939840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -700,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44810624"/>
+        <c:axId val="121939840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,7 +711,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40565376"/>
+        <c:crossAx val="121938304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,7 +736,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -970,11 +970,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="46327296"/>
-        <c:axId val="46328832"/>
+        <c:axId val="136846336"/>
+        <c:axId val="136852224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46327296"/>
+        <c:axId val="136846336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46328832"/>
+        <c:crossAx val="136852224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -991,7 +991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46328832"/>
+        <c:axId val="136852224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46327296"/>
+        <c:crossAx val="136846336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1027,7 +1027,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1261,11 +1261,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="47854720"/>
-        <c:axId val="47856256"/>
+        <c:axId val="136882048"/>
+        <c:axId val="136883584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47854720"/>
+        <c:axId val="136882048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47856256"/>
+        <c:crossAx val="136883584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1282,7 +1282,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47856256"/>
+        <c:axId val="136883584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47854720"/>
+        <c:crossAx val="136882048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1700,7 +1700,7 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection sqref="A1:F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>